<commit_message>
cleared data.xlsx this time for real
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mirek\IdeaProjects\GetDataFromWorkPortals\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A59479A-22FE-4007-B5DC-30B6C7D9823A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608C9697-283B-47AE-A2F8-16B45643AE55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{E4C8D30A-BB96-4518-832A-65DDBDCBD732}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>TIMESTAMP</t>
   </si>
@@ -82,34 +82,12 @@
   </si>
   <si>
     <t>ZADAVATEL</t>
-  </si>
-  <si>
-    <t>06.04.2021 14:49</t>
-  </si>
-  <si>
-    <t>jobs.cz</t>
-  </si>
-  <si>
-    <t>Junior IT Specialist</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>https://www.jobs.cz/rpd/1557615309/</t>
-  </si>
-  <si>
-    <t>Možnost občasné práce z domova</t>
-  </si>
-  <si>
-    <t>YES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,29 +434,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9B2CFC-478A-4BBD-9936-02EEE9F01803}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="63.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="41.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="44.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.5703125" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="23.7109375" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.5703125" collapsed="false"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="26.5703125" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="29.0" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="24.5703125" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.28515625" collapsed="false"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="63" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="44.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -532,59 +510,6 @@
       </c>
       <c r="Q1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed ExcelWriter so that is works with more columns in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mirek\IdeaProjects\GetDataFromWorkPortals\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608C9697-283B-47AE-A2F8-16B45643AE55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43C9F1E-0662-41D9-B1AC-B801D5F1175A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{E4C8D30A-BB96-4518-832A-65DDBDCBD732}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,14 +449,16 @@
     <col min="5" max="5" width="44.7109375" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="66.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="49.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="174.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="43.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="68.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
switch added to determine position level to jobspage
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mirek\IdeaProjects\GetDataFromWorkPortals\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8699E6DF-A30B-42F3-B4EB-36CB12EB8FB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA8FA2C-031E-4BC5-AB30-92137F44BCBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4C8D30A-BB96-4518-832A-65DDBDCBD732}"/>
   </bookViews>
@@ -453,8 +453,8 @@
     <col min="9" max="9" width="66.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="49.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="61.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="78.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="67.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="34.140625" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="43.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="29" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="68.28515625" bestFit="1" customWidth="1" collapsed="1"/>

</xml_diff>

<commit_message>
'delka pracovniho pomeru' a 'zarazeno' column deleted from excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mirek\IdeaProjects\GetDataFromWorkPortals\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA8FA2C-031E-4BC5-AB30-92137F44BCBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A9BE7E-0918-4CBF-B558-47F80E151A08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4C8D30A-BB96-4518-832A-65DDBDCBD732}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>TIMESTAMP</t>
   </si>
@@ -69,13 +69,7 @@
     <t>BENEFITY</t>
   </si>
   <si>
-    <t>ZAŘAZENO</t>
-  </si>
-  <si>
     <t>TYP_PRACOVNÍHO_POMĚRU</t>
-  </si>
-  <si>
-    <t>DÉLKA_PRACOVNÍHO_POMĚRU</t>
   </si>
   <si>
     <t>TYP_SMLUVNÍHO_VZTAHU</t>
@@ -434,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9B2CFC-478A-4BBD-9936-02EEE9F01803}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,14 +448,12 @@
     <col min="10" max="10" width="49.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="67.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="43.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="68.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="43.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="68.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,12 +498,6 @@
       </c>
       <c r="O1" t="s">
         <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new data in excel files
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mirek\IdeaProjects\GetDataFromWorkPortals\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A9BE7E-0918-4CBF-B558-47F80E151A08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF5F0BC-78C1-4816-BC71-25C9971D4EEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4C8D30A-BB96-4518-832A-65DDBDCBD732}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>TIMESTAMP</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>ZADAVATEL</t>
+  </si>
+  <si>
+    <t>KONTAKTNÍ_OSOBA</t>
+  </si>
+  <si>
+    <t>KONTAKTNÍ_INFO</t>
   </si>
 </sst>
 </file>
@@ -428,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9B2CFC-478A-4BBD-9936-02EEE9F01803}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,16 +450,18 @@
     <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="66.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="49.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="67.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="43.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="68.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="66.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="49.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="67.140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="43.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="68.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,24 +487,30 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
setting up filter finished
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mirek\IdeaProjects\GetDataFromWorkPortals\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF5F0BC-78C1-4816-BC71-25C9971D4EEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A0B061-50F3-4F15-98E8-EDB29A45E110}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4C8D30A-BB96-4518-832A-65DDBDCBD732}"/>
   </bookViews>

</xml_diff>